<commit_message>
Fix 'Rejeter avenant' issue
</commit_message>
<xml_diff>
--- a/download/les maquettes DGI/les fichiers excel/annex 2/maquette_teledeclaration_2022.xlsx
+++ b/download/les maquettes DGI/les fichiers excel/annex 2/maquette_teledeclaration_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -420,22 +420,22 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>IF1</v>
+        <v/>
       </c>
       <c r="B2" t="str">
-        <v>F4767464</v>
+        <v>K5443645</v>
       </c>
       <c r="C2" t="str">
         <v/>
       </c>
       <c r="D2" t="str">
-        <v xml:space="preserve">MED FARID </v>
+        <v>KHADIJA LALA</v>
       </c>
       <c r="E2" t="str">
-        <v>OIUJOIIP345654</v>
+        <v>KHDEHOI35456</v>
       </c>
       <c r="F2" t="str">
-        <v>LJDJZALJ</v>
+        <v>AAAAAA</v>
       </c>
       <c r="G2" t="str">
         <v>LUC</v>
@@ -444,36 +444,36 @@
         <v>-</v>
       </c>
       <c r="I2" t="str">
-        <v>165000.00</v>
+        <v>100000.00</v>
       </c>
       <c r="J2" t="str">
-        <v>22500.00</v>
+        <v>13500.00</v>
       </c>
       <c r="K2" t="str">
-        <v>142500.00</v>
+        <v>86500.00</v>
       </c>
       <c r="L2" t="str">
-        <v>TSR.10.2018</v>
+        <v>TRS.15.2018</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>IF2</v>
+        <v/>
       </c>
       <c r="B3" t="str">
-        <v>K5443645</v>
+        <v>L3578354</v>
       </c>
       <c r="C3" t="str">
         <v/>
       </c>
       <c r="D3" t="str">
-        <v>KHADIJA LALA</v>
+        <v>NABIL KAMAL</v>
       </c>
       <c r="E3" t="str">
-        <v>KHDEHOI35456</v>
+        <v>PMLPL35434</v>
       </c>
       <c r="F3" t="str">
-        <v>FES PKPO2545454</v>
+        <v>WWWWW</v>
       </c>
       <c r="G3" t="str">
         <v>LUC</v>
@@ -482,36 +482,36 @@
         <v>-</v>
       </c>
       <c r="I3" t="str">
-        <v>33600.00</v>
+        <v>70000.00</v>
       </c>
       <c r="J3" t="str">
-        <v>2880.00</v>
+        <v>9000.00</v>
       </c>
       <c r="K3" t="str">
-        <v>30720.00</v>
+        <v>61000.00</v>
       </c>
       <c r="L3" t="str">
-        <v>TSR.10.2018</v>
+        <v>TRS.15.2018</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>IF3</v>
+        <v/>
       </c>
       <c r="B4" t="str">
-        <v>L3578354</v>
+        <v>D524564</v>
       </c>
       <c r="C4" t="str">
         <v/>
       </c>
       <c r="D4" t="str">
-        <v>NABIL KAMAL</v>
+        <v>SAMIRA TATA</v>
       </c>
       <c r="E4" t="str">
-        <v>PMLPL35434</v>
+        <v>LKJOIFEJIOZ</v>
       </c>
       <c r="F4" t="str">
-        <v>FES PKPO2545454</v>
+        <v>QW</v>
       </c>
       <c r="G4" t="str">
         <v>LUC</v>
@@ -520,21 +520,21 @@
         <v>-</v>
       </c>
       <c r="I4" t="str">
-        <v>50400.00</v>
+        <v>60000.00</v>
       </c>
       <c r="J4" t="str">
-        <v>4320.00</v>
+        <v>7500.00</v>
       </c>
       <c r="K4" t="str">
-        <v>46080.00</v>
+        <v>52500.00</v>
       </c>
       <c r="L4" t="str">
-        <v>TSR.10.2018</v>
+        <v>TRS.15.2018</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>IF4</v>
+        <v/>
       </c>
       <c r="B5" t="str">
         <v>P5874857</v>
@@ -549,7 +549,7 @@
         <v>FREGREG68796</v>
       </c>
       <c r="F5" t="str">
-        <v>LJODIEJ354</v>
+        <v>QQQQQQQQQ</v>
       </c>
       <c r="G5" t="str">
         <v>LUC</v>
@@ -558,92 +558,92 @@
         <v>-</v>
       </c>
       <c r="I5" t="str">
-        <v>200000.00</v>
+        <v>50000.00</v>
       </c>
       <c r="J5" t="str">
-        <v>30000.00</v>
+        <v>6000.00</v>
       </c>
       <c r="K5" t="str">
-        <v>170000.00</v>
+        <v>44000.00</v>
       </c>
       <c r="L5" t="str">
-        <v>TSR.10.2018</v>
+        <v>TRS.15.2018</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>IF5</v>
+        <v/>
       </c>
       <c r="B6" t="str">
-        <v>D524564</v>
+        <v/>
       </c>
       <c r="C6" t="str">
         <v/>
       </c>
       <c r="D6" t="str">
-        <v>SAMIRA TATA</v>
+        <v/>
       </c>
       <c r="E6" t="str">
-        <v>LKJOIFEJIOZ</v>
+        <v/>
       </c>
       <c r="F6" t="str">
-        <v>JKHIOHOI1354654</v>
+        <v/>
       </c>
       <c r="G6" t="str">
-        <v>LUC</v>
+        <v/>
       </c>
       <c r="H6" t="str">
-        <v>-</v>
+        <v/>
       </c>
       <c r="I6" t="str">
-        <v>200000.00</v>
+        <v/>
       </c>
       <c r="J6" t="str">
-        <v>25500.00</v>
+        <v/>
       </c>
       <c r="K6" t="str">
-        <v>174500.00</v>
+        <v/>
       </c>
       <c r="L6" t="str">
-        <v>TSR.10.2018</v>
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>IF6</v>
+        <v/>
       </c>
       <c r="B7" t="str">
-        <v>BJ110393</v>
+        <v/>
       </c>
       <c r="C7" t="str">
         <v/>
       </c>
       <c r="D7" t="str">
-        <v>TRM TEST</v>
+        <v>identifiantFiscal</v>
       </c>
       <c r="E7" t="str">
-        <v>TEST</v>
+        <v>exerciceFiscalDu</v>
       </c>
       <c r="F7" t="str">
-        <v>TEST</v>
+        <v>exerciceFiscalAu</v>
       </c>
       <c r="G7" t="str">
-        <v>LUC</v>
+        <v>annee</v>
       </c>
       <c r="H7" t="str">
-        <v>-</v>
+        <v>totalMntBrutLoyer</v>
       </c>
       <c r="I7" t="str">
-        <v>30000.00</v>
+        <v>totalMntRetenueSource</v>
       </c>
       <c r="J7" t="str">
-        <v>3000.00</v>
+        <v>totalMntNetLoyer</v>
       </c>
       <c r="K7" t="str">
-        <v>27000.00</v>
+        <v/>
       </c>
       <c r="L7" t="str">
-        <v>TSR.10.2018</v>
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -657,112 +657,36 @@
         <v/>
       </c>
       <c r="D8" t="str">
-        <v/>
+        <v>IF</v>
       </c>
       <c r="E8" t="str">
-        <v/>
+        <v>2022-01-01</v>
       </c>
       <c r="F8" t="str">
-        <v/>
+        <v>2022-12-31</v>
       </c>
       <c r="G8" t="str">
-        <v/>
+        <v>2022</v>
       </c>
       <c r="H8" t="str">
-        <v/>
+        <v>280000.00</v>
       </c>
       <c r="I8" t="str">
-        <v/>
+        <v>36000.00</v>
       </c>
       <c r="J8" t="str">
-        <v/>
+        <v>244000.00</v>
       </c>
       <c r="K8" t="str">
         <v/>
       </c>
       <c r="L8" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v/>
-      </c>
-      <c r="B9" t="str">
-        <v/>
-      </c>
-      <c r="C9" t="str">
-        <v/>
-      </c>
-      <c r="D9" t="str">
-        <v>identifiantFiscal</v>
-      </c>
-      <c r="E9" t="str">
-        <v>exerciceFiscalDu</v>
-      </c>
-      <c r="F9" t="str">
-        <v>exerciceFiscalAu</v>
-      </c>
-      <c r="G9" t="str">
-        <v>annee</v>
-      </c>
-      <c r="H9" t="str">
-        <v>totalMntBrutLoyer</v>
-      </c>
-      <c r="I9" t="str">
-        <v>totalMntRetenueSource</v>
-      </c>
-      <c r="J9" t="str">
-        <v>totalMntNetLoyer</v>
-      </c>
-      <c r="K9" t="str">
-        <v/>
-      </c>
-      <c r="L9" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v/>
-      </c>
-      <c r="B10" t="str">
-        <v/>
-      </c>
-      <c r="C10" t="str">
-        <v/>
-      </c>
-      <c r="D10" t="str">
-        <v>IF</v>
-      </c>
-      <c r="E10" t="str">
-        <v>2022-01-01</v>
-      </c>
-      <c r="F10" t="str">
-        <v>2022-12-31</v>
-      </c>
-      <c r="G10" t="str">
-        <v>2022</v>
-      </c>
-      <c r="H10" t="str">
-        <v>679000.00</v>
-      </c>
-      <c r="I10" t="str">
-        <v>88200.00</v>
-      </c>
-      <c r="J10" t="str">
-        <v>590800.00</v>
-      </c>
-      <c r="K10" t="str">
-        <v/>
-      </c>
-      <c r="L10" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>